<commit_message>
Ajouts de données de table
</commit_message>
<xml_diff>
--- a/conf/Table_Aptitudes_Type_aptitudes_Caracteristique_JDR_2R.xlsx
+++ b/conf/Table_Aptitudes_Type_aptitudes_Caracteristique_JDR_2R.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Projets\jdr2d\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE58D61-1184-41E3-9B02-4BF8E7B34FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528CC36-DACC-46EA-9042-2308D76FE940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34F6F82D-5E26-4D0F-A51F-90A17C34A5CE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{34F6F82D-5E26-4D0F-A51F-90A17C34A5CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Aptitude" sheetId="2" r:id="rId2"/>
+    <sheet name="Caractéristique" sheetId="3" r:id="rId3"/>
+    <sheet name="Type_aptitude" sheetId="4" r:id="rId4"/>
+    <sheet name="Lieu" sheetId="5" r:id="rId5"/>
+    <sheet name="Objectif" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="197">
   <si>
     <t>type_aptitude</t>
   </si>
@@ -421,6 +425,210 @@
   </si>
   <si>
     <t>plante une graine sur une cible allié et la soigne sur la durée pdt 10 sec OU une cible ennemie et lui inflige des dgt de nature sur la durée pdt 5 sec</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>LIEU</t>
+  </si>
+  <si>
+    <t>id_lieu</t>
+  </si>
+  <si>
+    <t>nom_lieu</t>
+  </si>
+  <si>
+    <t>description_lieu</t>
+  </si>
+  <si>
+    <t>carte_lieu</t>
+  </si>
+  <si>
+    <t>Bad-town</t>
+  </si>
+  <si>
+    <t>la reine</t>
+  </si>
+  <si>
+    <t>la bête</t>
+  </si>
+  <si>
+    <t>scissor palace</t>
+  </si>
+  <si>
+    <t>lennybar</t>
+  </si>
+  <si>
+    <t>Profit-city</t>
+  </si>
+  <si>
+    <t>black market</t>
+  </si>
+  <si>
+    <t>lehman sisters</t>
+  </si>
+  <si>
+    <t>place-2-B</t>
+  </si>
+  <si>
+    <t>treump shop</t>
+  </si>
+  <si>
+    <t>Nainportnawak</t>
+  </si>
+  <si>
+    <t>maxilase</t>
+  </si>
+  <si>
+    <t>flunchbar</t>
+  </si>
+  <si>
+    <t>park in son</t>
+  </si>
+  <si>
+    <t>in &amp; out</t>
+  </si>
+  <si>
+    <t>Elf village</t>
+  </si>
+  <si>
+    <t>msncircus</t>
+  </si>
+  <si>
+    <t>pirate search</t>
+  </si>
+  <si>
+    <t>daddy awards</t>
+  </si>
+  <si>
+    <t>potatoe valley</t>
+  </si>
+  <si>
+    <t>La croisée</t>
+  </si>
+  <si>
+    <t>Ville des orcs</t>
+  </si>
+  <si>
+    <t>Lieu de combat n°1</t>
+  </si>
+  <si>
+    <t>Centre de pari sur les combats</t>
+  </si>
+  <si>
+    <t>Un casino</t>
+  </si>
+  <si>
+    <t>La taverne, idéal pour s''amuser</t>
+  </si>
+  <si>
+    <t>Ville des humains</t>
+  </si>
+  <si>
+    <t>Le marché : pour acheter, vendre et échanger</t>
+  </si>
+  <si>
+    <t>La banque</t>
+  </si>
+  <si>
+    <t>La place centrale de la ville</t>
+  </si>
+  <si>
+    <t>Magasin d''armures</t>
+  </si>
+  <si>
+    <t>Ville des nains</t>
+  </si>
+  <si>
+    <t>Magasin de potions</t>
+  </si>
+  <si>
+    <t>La taverne des nains, l''alccol coule à flot !</t>
+  </si>
+  <si>
+    <t>Joli parc pour ce détendre</t>
+  </si>
+  <si>
+    <t>Restaurant de spécialités locales</t>
+  </si>
+  <si>
+    <t>Ville des elfes</t>
+  </si>
+  <si>
+    <t>Place pour discuter et faire des rencontres</t>
+  </si>
+  <si>
+    <t>Zone pour aller chercher de nouvelles quêtes</t>
+  </si>
+  <si>
+    <t>Centre de récompences pour les quêtes</t>
+  </si>
+  <si>
+    <t>Potager de légumes</t>
+  </si>
+  <si>
+    <t>Là où tout les chemins se croisent</t>
+  </si>
+  <si>
+    <t>OBJECTIF</t>
+  </si>
+  <si>
+    <t>id_objectif</t>
+  </si>
+  <si>
+    <t>nom_objectif</t>
+  </si>
+  <si>
+    <t>description_objectif</t>
+  </si>
+  <si>
+    <t>validation_objectif</t>
+  </si>
+  <si>
+    <t>recuperer du houblon (Alain Chichon)</t>
+  </si>
+  <si>
+    <t>recuperer un fut (Maitre Kanter)</t>
+  </si>
+  <si>
+    <t>recuperer un élement secret (Chie mi Hendrix)</t>
+  </si>
+  <si>
+    <t>Aller tuer 4 chauves souris</t>
+  </si>
+  <si>
+    <t>Aller recuperer l''arme chez Durdur</t>
+  </si>
+  <si>
+    <t>Tuer Dracula (Jean Marie le PNJ)</t>
+  </si>
+  <si>
+    <t>Aller voir Hippique-sous pour avoir des infos</t>
+  </si>
+  <si>
+    <t>Donner des sousous à Durdur pour avoir une casquette à pointe afin de récupérer une boubourse à son concours de lancer de pommes</t>
+  </si>
+  <si>
+    <t>Retourner voir Benard Tappir et lui donner la boubourse gagner au concours de lancer de pomme</t>
+  </si>
+  <si>
+    <t>Combattre à l''arene</t>
+  </si>
+  <si>
+    <t>Choisir de tuer ou non Bours-La</t>
+  </si>
+  <si>
+    <t>Aller voir Nana Moule Curry pour récuperer la potion() a vendu la derniere potion au casino) elle lui donne une musse tongue à la place</t>
+  </si>
+  <si>
+    <t>rejoindre Lost Vegas au Scissor Palace</t>
+  </si>
+  <si>
+    <t>visiter le tunnel du pont en musse tongue avec Die Anna</t>
   </si>
 </sst>
 </file>
@@ -519,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,15 +735,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,6 +755,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2945,1068 +3160,692 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4908D6-739E-487D-92BB-5EB515A84962}">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="7"/>
-      <c r="R1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="12"/>
+      <c r="A1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="9"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="12"/>
-      <c r="R2" s="11" t="s">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="8">
+        <v>1</v>
+      </c>
+      <c r="V3" s="9"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="8">
+        <v>1</v>
+      </c>
+      <c r="V4" s="9"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="U2" s="12"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="B5" s="13"/>
+      <c r="C5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
-      <c r="R3" s="11">
+      <c r="V5" s="9"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="8">
         <v>1</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="U3" s="10"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="8">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="8">
+        <v>1</v>
+      </c>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="8">
+        <v>1</v>
+      </c>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="10"/>
-      <c r="R4" s="11">
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="8">
         <v>2</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="U4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="8">
+        <v>2</v>
+      </c>
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="8">
+        <v>2</v>
+      </c>
+      <c r="V14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="8">
+        <v>2</v>
+      </c>
+      <c r="V15" s="9"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
-      <c r="R5" s="11">
+      <c r="V16" s="9"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="8">
         <v>3</v>
       </c>
-      <c r="S5" s="12"/>
-      <c r="T5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="U5" s="10"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="8">
+        <v>3</v>
+      </c>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
-      <c r="R6" s="11">
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>18</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="8">
         <v>4</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="U6" s="10"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="12"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="V14" s="12"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>1</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="11">
-        <v>1</v>
-      </c>
-      <c r="V15" s="12"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>2</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="11">
-        <v>1</v>
-      </c>
-      <c r="V16" s="12"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>3</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="11">
-        <v>1</v>
-      </c>
-      <c r="V17" s="12"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
-        <v>4</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="11">
-        <v>1</v>
-      </c>
-      <c r="V18" s="12"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <v>5</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="11">
-        <v>1</v>
-      </c>
-      <c r="V19" s="12"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
-        <v>6</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="11">
-        <v>1</v>
-      </c>
-      <c r="V20" s="12"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <v>7</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="11">
-        <v>1</v>
-      </c>
-      <c r="V21" s="12"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>8</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="11">
-        <v>1</v>
-      </c>
-      <c r="V22" s="12"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
-        <v>9</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="11">
-        <v>2</v>
-      </c>
-      <c r="V23" s="12"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>10</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="11">
-        <v>2</v>
-      </c>
-      <c r="V24" s="12"/>
+      <c r="V20" s="9"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>11</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="11">
-        <v>2</v>
-      </c>
-      <c r="V25" s="12"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>12</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="11">
-        <v>2</v>
-      </c>
-      <c r="V26" s="12"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
-        <v>13</v>
-      </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="11">
-        <v>2</v>
-      </c>
-      <c r="V27" s="12"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
-        <v>14</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="11">
-        <v>3</v>
-      </c>
-      <c r="V28" s="12"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
-        <v>15</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="11">
-        <v>3</v>
-      </c>
-      <c r="V29" s="12"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
-        <v>16</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="11">
-        <v>3</v>
-      </c>
-      <c r="V30" s="12"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>17</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="11">
-        <v>4</v>
-      </c>
-      <c r="V31" s="12"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
-        <v>18</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="11">
-        <v>4</v>
-      </c>
-      <c r="V32" s="12"/>
+      <c r="G25" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="154">
-    <mergeCell ref="I22:T22"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I14:T14"/>
-    <mergeCell ref="I15:T15"/>
-    <mergeCell ref="I16:T16"/>
-    <mergeCell ref="I17:T17"/>
-    <mergeCell ref="I18:T18"/>
-    <mergeCell ref="I19:T19"/>
-    <mergeCell ref="I20:T20"/>
-    <mergeCell ref="I21:T21"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A13:V13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="I23:T23"/>
-    <mergeCell ref="I24:T24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="I32:T32"/>
-    <mergeCell ref="I26:T26"/>
-    <mergeCell ref="I27:T27"/>
-    <mergeCell ref="I28:T28"/>
-    <mergeCell ref="I29:T29"/>
-    <mergeCell ref="I30:T30"/>
-    <mergeCell ref="I31:T31"/>
-    <mergeCell ref="I25:T25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="E6:P6"/>
-    <mergeCell ref="E7:P7"/>
-    <mergeCell ref="E8:P8"/>
-    <mergeCell ref="E9:P9"/>
-    <mergeCell ref="E10:P10"/>
+  <mergeCells count="115">
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I3:T3"/>
+    <mergeCell ref="I4:T4"/>
+    <mergeCell ref="I5:T5"/>
+    <mergeCell ref="I6:T6"/>
+    <mergeCell ref="I7:T7"/>
+    <mergeCell ref="I8:T8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
@@ -4019,18 +3858,1549 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="I20:T20"/>
+    <mergeCell ref="I14:T14"/>
+    <mergeCell ref="I15:T15"/>
+    <mergeCell ref="I16:T16"/>
+    <mergeCell ref="I17:T17"/>
+    <mergeCell ref="I18:T18"/>
+    <mergeCell ref="I19:T19"/>
+    <mergeCell ref="I13:T13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I11:T11"/>
+    <mergeCell ref="I12:T12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I9:T9"/>
+    <mergeCell ref="I10:T10"/>
+    <mergeCell ref="U9:V9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB608F9-2173-40A5-A1E8-A4A15644AA90}">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:P10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:P8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:P9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:P6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:P7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:P4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:P5"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="E3:P3"/>
-    <mergeCell ref="E4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE3506-FD41-4146-93F4-2CE3BF7C175F}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0028CF7F-1952-4BDC-8711-26B3376B7164}">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="6" max="7" width="10" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="15"/>
+      <c r="K3" t="str">
+        <f>A2&amp;", "&amp;B2&amp;", "&amp;D2&amp;", "&amp;H2</f>
+        <v>id_lieu, nom_lieu, description_lieu, carte_lieu</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="15"/>
+      <c r="J4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" t="str">
+        <f>(A3&amp;", '"&amp;B3&amp;"', '"&amp;D3)</f>
+        <v>1, 'Bad-town', 'Ville des orcs</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="15"/>
+      <c r="J5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" t="str">
+        <f>(A4&amp;", '"&amp;B4&amp;"', '"&amp;D4)</f>
+        <v>2, 'la reine', 'Lieu de combat n°1</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="15"/>
+      <c r="J6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" t="str">
+        <f>(A5&amp;", '"&amp;B5&amp;"', '"&amp;D5)</f>
+        <v>3, 'la bête', 'Centre de pari sur les combats</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="15"/>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" t="str">
+        <f>(A6&amp;", '"&amp;B6&amp;"', '"&amp;D6)</f>
+        <v>4, 'scissor palace', 'Un casino</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="15"/>
+      <c r="J8" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" t="str">
+        <f>(A7&amp;", '"&amp;B7&amp;"', '"&amp;D7)</f>
+        <v>5, 'lennybar', 'La taverne, idéal pour s''amuser</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="15"/>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" t="str">
+        <f>(A8&amp;", '"&amp;B8&amp;"', '"&amp;D8)</f>
+        <v>6, 'Profit-city', 'Ville des humains</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="15"/>
+      <c r="J10" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" t="str">
+        <f>(A9&amp;", '"&amp;B9&amp;"', '"&amp;D9)</f>
+        <v>7, 'black market', 'Le marché : pour acheter, vendre et échanger</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="15"/>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" t="str">
+        <f>(A10&amp;", '"&amp;B10&amp;"', '"&amp;D10)</f>
+        <v>8, 'lehman sisters', 'La banque</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="15"/>
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" t="str">
+        <f>(A11&amp;", '"&amp;B11&amp;"', '"&amp;D11)</f>
+        <v>9, 'place-2-B', 'La place centrale de la ville</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="15"/>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" t="str">
+        <f>(A12&amp;", '"&amp;B12&amp;"', '"&amp;D12)</f>
+        <v>10, 'treump shop', 'Magasin d''armures</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="15"/>
+      <c r="J14" t="s">
+        <v>129</v>
+      </c>
+      <c r="K14" t="str">
+        <f>(A13&amp;", '"&amp;B13&amp;"', '"&amp;D13)</f>
+        <v>11, 'Nainportnawak', 'Ville des nains</v>
+      </c>
+      <c r="P14" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="15"/>
+      <c r="J15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" t="str">
+        <f>(A14&amp;", '"&amp;B14&amp;"', '"&amp;D14)</f>
+        <v>12, 'maxilase', 'Magasin de potions</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="15"/>
+      <c r="J16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K16" t="str">
+        <f>(A15&amp;", '"&amp;B15&amp;"', '"&amp;D15)</f>
+        <v>13, 'flunchbar', 'La taverne des nains, l''alccol coule à flot !</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="15"/>
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+      <c r="K17" t="str">
+        <f>(A16&amp;", '"&amp;B16&amp;"', '"&amp;D16)</f>
+        <v>14, 'park in son', 'Joli parc pour ce détendre</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="15"/>
+      <c r="J18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K18" t="str">
+        <f>(A17&amp;", '"&amp;B17&amp;"', '"&amp;D17)</f>
+        <v>15, 'in &amp; out', 'Restaurant de spécialités locales</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="15"/>
+      <c r="J19" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" t="str">
+        <f>(A18&amp;", '"&amp;B18&amp;"', '"&amp;D18)</f>
+        <v>16, 'Elf village', 'Ville des elfes</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="15"/>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" t="str">
+        <f>(A19&amp;", '"&amp;B19&amp;"', '"&amp;D19)</f>
+        <v>17, 'msncircus', 'Place pour discuter et faire des rencontres</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="15"/>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+      <c r="K21" t="str">
+        <f>(A20&amp;", '"&amp;B20&amp;"', '"&amp;D20)</f>
+        <v>18, 'pirate search', 'Zone pour aller chercher de nouvelles quêtes</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="15"/>
+      <c r="J22" t="s">
+        <v>129</v>
+      </c>
+      <c r="K22" t="str">
+        <f>(A21&amp;", '"&amp;B21&amp;"', '"&amp;D21)</f>
+        <v>19, 'daddy awards', 'Centre de récompences pour les quêtes</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="15"/>
+      <c r="J23" t="s">
+        <v>129</v>
+      </c>
+      <c r="K23" t="str">
+        <f>(A22&amp;", '"&amp;B22&amp;"', '"&amp;D22)</f>
+        <v>20, 'potatoe valley', 'Potager de légumes</v>
+      </c>
+      <c r="P23" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" t="str">
+        <f>(A23&amp;", '"&amp;B23&amp;"', '"&amp;D23)</f>
+        <v>21, 'La croisée', 'Là où tout les chemins se croisent</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="45">
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577DA391-A061-463E-9151-E75A84D4AE68}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="P2" s="13"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="13"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="13"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="13"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="13"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="13"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P16" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="D13:N13"/>
+    <mergeCell ref="D14:N14"/>
+    <mergeCell ref="D15:N15"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="D7:N7"/>
+    <mergeCell ref="D8:N8"/>
+    <mergeCell ref="D9:N9"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="D11:N11"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="D3:N3"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="D6:N6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>